<commit_message>
finalized board checked all errors
</commit_message>
<xml_diff>
--- a/GerberandDrillTop/BOM/Copy of Bill of Materials-RPD_top.xlsx
+++ b/GerberandDrillTop/BOM/Copy of Bill of Materials-RPD_top.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{489377E4-46FB-45D5-BAB4-F7D2109CDDDC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{141B20D8-B3A6-494D-B8D5-34652DCAA89A}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of Bill of Materials-RPD_t" sheetId="1" r:id="rId1"/>
@@ -668,7 +668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FF8630-41C0-4FA2-A1A8-FE752B69E96D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F3F499-75D3-4D54-9C24-082BB64B50B5}">
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
added ams status and imd status, re-routed and re-generated
</commit_message>
<xml_diff>
--- a/GerberandDrillTop/BOM/Copy of Bill of Materials-RPD_top.xlsx
+++ b/GerberandDrillTop/BOM/Copy of Bill of Materials-RPD_top.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{141B20D8-B3A6-494D-B8D5-34652DCAA89A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{FE38DCFE-35E7-45F6-84FC-E98E3861B407}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of Bill of Materials-RPD_t" sheetId="1" r:id="rId1"/>
@@ -668,7 +668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F3F499-75D3-4D54-9C24-082BB64B50B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0670F5E-1355-4F83-8B69-A37832FDB62E}">
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>